<commit_message>
Custom Sort, Search implemented
</commit_message>
<xml_diff>
--- a/Alldbs.xlsx
+++ b/Alldbs.xlsx
@@ -9,29 +9,36 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="803" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="803" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="0" sheetId="1" r:id="rId1"/>
     <sheet name="Subas" sheetId="2" r:id="rId2"/>
+    <sheet name="Jersey" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t xml:space="preserve">Info </t>
-  </si>
-  <si>
-    <t>Added new Items at2022-01-24T22:32:49.059155500</t>
-  </si>
-  <si>
-    <t>Opened on 2022-01-24T22:33:00.045086900</t>
-  </si>
-  <si>
-    <t>Opened on 2022-01-24T22:33:00.941689200</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Deleted an Item on  2022-01-28T11:10:48.930609900</t>
+  </si>
+  <si>
+    <t>Opened on 2022-01-28T12:39:27.616090300</t>
+  </si>
+  <si>
+    <t>Deleted an Item on  2022-01-28T12:39:27.640024800</t>
+  </si>
+  <si>
+    <t>Opened on 2022-01-28T12:39:32.222596700</t>
+  </si>
+  <si>
+    <t>Opened on 2022-01-28T12:40:43.089242300</t>
+  </si>
+  <si>
+    <t>Opened on 2022-01-28T12:40:46.383302400</t>
   </si>
 </sst>
 </file>
@@ -364,7 +371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -372,10 +379,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>